<commit_message>
Update brewery list for 2024
</commit_message>
<xml_diff>
--- a/breweryData/ListOfBreweriesAndBeers.xlsx
+++ b/breweryData/ListOfBreweriesAndBeers.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikolaszagarella/venvs/Personal/RochesterBeerExpo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikolaszagarella/venvs/Personal/rochester-beer-search/breweryData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0A5F897-CD89-9D4E-A73B-8A12FC85C1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3269B50B-27A2-E045-899D-54DE63297BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21500" yWindow="7780" windowWidth="28040" windowHeight="17440" xr2:uid="{F905F144-C3AC-D947-85A6-6FED96429477}"/>
+    <workbookView xWindow="7960" yWindow="4180" windowWidth="28040" windowHeight="17440" xr2:uid="{F905F144-C3AC-D947-85A6-6FED96429477}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2024" sheetId="2" r:id="rId1"/>
+    <sheet name="2023" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="330">
   <si>
     <t>Rohrbach Brewing</t>
   </si>
@@ -481,13 +482,556 @@
   </si>
   <si>
     <t>Beers</t>
+  </si>
+  <si>
+    <t> Kilt Switch Scotch ale; Texas imperial Pils; Hurricane Slushy Berliner; Dr. Seltzer hard seltzer;</t>
+  </si>
+  <si>
+    <t> Rocky Road imperial sweet stout; Tee Time Berliner; Zest in Peace wheat ale;</t>
+  </si>
+  <si>
+    <t> Cold brew coffee; Espresso *NA*;</t>
+  </si>
+  <si>
+    <t> Summer Farm Ale; Hibiscus Passionfruit Sour; Dubbel;</t>
+  </si>
+  <si>
+    <t> Sunnyside DIPA; Grandma Fingers blueberry cobbler sour;</t>
+  </si>
+  <si>
+    <t> Mexican lager; Seasonal TBA *NA*;</t>
+  </si>
+  <si>
+    <t> Blumen IPA; White Chocolate Cherry Berry Blender sour;</t>
+  </si>
+  <si>
+    <t> Baby Kiwi pale ale; Distorted Re(ale)ity pale ale;</t>
+  </si>
+  <si>
+    <t> Hard seltzers, Limeade; Moscado Lemonade; Blood Orange Punch;</t>
+  </si>
+  <si>
+    <t> Pineapple Burner IPA; Strawberry Vision sour; West Coast Burner IPA; Natural Blonde Belgian blonde;</t>
+  </si>
+  <si>
+    <t> Archimedes Belgian dark strong; Mexican lager; Falcon NEIPA;</t>
+  </si>
+  <si>
+    <t> Cluster Honey cider; Summer cider (strawberry prickly pear);</t>
+  </si>
+  <si>
+    <t> Reverend Kane Rum Barrel Aged Imperial Stout; Blood Light pale ale; Bloodvar Czech Pils; Stone Fruit Steve Austin session cherry blackberry sour;</t>
+  </si>
+  <si>
+    <t> Serum-S025 pineapple coconut session mead; Blueberry pomegranate session mead; Serum-S017.1 fruit punch;</t>
+  </si>
+  <si>
+    <t> 8 Hour Custom NEIPA; Savages Kolsch; Punch Bowl (peaches &amp; cream) sour;</t>
+  </si>
+  <si>
+    <t> Coalport Czech dark, Helles (German gravity keg!);</t>
+  </si>
+  <si>
+    <t> Hex Hefeweizen; Into the Underdark blackberry mojito sour;</t>
+  </si>
+  <si>
+    <t> Chaotic Orbit NEIPA; Chat Room WC Pils; Odysseus TIPA;</t>
+  </si>
+  <si>
+    <t> Cindi's Hard Mountain Tea; Lil Cinder Light Lime; Mango Breaker (sour mango IPA);</t>
+  </si>
+  <si>
+    <t> Mamba hazy DIPA; Breathe hazy IPA; Zombie (Black currant, mango, coconut cream) smoothie sour; BA treats;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TBA;</t>
+  </si>
+  <si>
+    <t> Strawberry Pretzel Salad Gose; El Trono Mexican lager; Double Your Circuits DIPA; Secret Machine</t>
+  </si>
+  <si>
+    <t> The Final Cap blended BA beer; tba;</t>
+  </si>
+  <si>
+    <t> Taste of Paradise; Strawberry Rhubarb; The Batch;</t>
+  </si>
+  <si>
+    <t> Just Be Helles lager; Over Zealous DIPA; The Usual IPA;</t>
+  </si>
+  <si>
+    <t> Intrepid blonde stout; For Elise Vienna lager; Holle's Little Pilsner;</t>
+  </si>
+  <si>
+    <t> Eugene's Axe DIPA; Roaming with Fireflies IPA;</t>
+  </si>
+  <si>
+    <t> Dizzny Blizzy heavily fruited sour; Up the Road DIPA; Lucerna Czech Pils;</t>
+  </si>
+  <si>
+    <t> Little Coconut snacky imperial stout; Whale Watching DIPA; Smooth Beats Miami coconut IPA;</t>
+  </si>
+  <si>
+    <t> Natural Flavors Strawberry sour IPA; Just Fruit Peach Mango heavily fruited sour; Get Pitted (light lager with fruits of the sun);</t>
+  </si>
+  <si>
+    <t> Juice Life IPA; Concord Grape Liquid Lollipop heavily fruited sour;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GBH Helles; Alora Cream Ale; 12 Horse;</t>
+  </si>
+  <si>
+    <t> The Open Work</t>
+  </si>
+  <si>
+    <t> The Wilds Hazy IPA; Haus Effect lager (LUKR pour); BA A Dark Bloom imperial stout with coconut;</t>
+  </si>
+  <si>
+    <t> Sun Wukong (Chinese green tea ferment); Lapsang Souchong (smoked Chinese black tea); Chimera (green + white tea blend); Echinacea. (NA);</t>
+  </si>
+  <si>
+    <t> THYKK mango lassi sour; LUUV pineapple whip sour; LUUV orange whip sour; Drowning Clown DIPA;</t>
+  </si>
+  <si>
+    <t>  Polotmavy Czech amber lager;</t>
+  </si>
+  <si>
+    <t> Maple Bourbon Grapefruit; Soda Series</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chem Trails;</t>
+  </si>
+  <si>
+    <t> Banana Nirvana imperial stout; Schmoojee Patisserree Raspberry Cheesecake smoothie sour; Gloopfellas Schmoojee smootie sour; Sun Lust hazy DIPA;</t>
+  </si>
+  <si>
+    <t> Dry-hopped Cream Ale; Shore Leave Pineapple Upside Down Cake sour; Barley One BA barleywine; Avast! blueberry cobbler sour;</t>
+  </si>
+  <si>
+    <t> Espresso Three Shores almond stout; No Filter</t>
+  </si>
+  <si>
+    <t>  Porch Fest lager; Bella Lago Italian Pils;</t>
+  </si>
+  <si>
+    <t>  K2 lite (with fruit); Kylix NEIPA; Raspberry Lemonade Sour; Spicy Bloody Mary Dill Pickle Sour;</t>
+  </si>
+  <si>
+    <t> Two seasonal flavors (*NA*);</t>
+  </si>
+  <si>
+    <t> Pulpy IPA; Pulp Up The Late Night Jams imperial sour (Definitive collab); Cereal Killer imperial stout; No Time To Die TIPA (Modestman collab);</t>
+  </si>
+  <si>
+    <t> Basil lemon blueberry hard seltzer; new hazy IPA;</t>
+  </si>
+  <si>
+    <t> Penn Yan Ice; TBA;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mix of FLX and Australian wines;</t>
+  </si>
+  <si>
+    <t> No Wake (orange pineapple sour aged in gin barrel); Mixed berry hard seltzer;</t>
+  </si>
+  <si>
+    <t> Juice Lord hazy DIPA; Green Place IPA; Dark Messenger vanilla porter; Never Ending Game DIPA;</t>
+  </si>
+  <si>
+    <t> Hazy Headlines IPA; Oni Giri rice lager; Cleveland Experiment, Vol. 3 hazy IPA; Lizard People, Dear Reader hazy DIPA;</t>
+  </si>
+  <si>
+    <t> Memento Mori Mild with Earl Grey; Janky IPA; Dapper Vienna Lager;</t>
+  </si>
+  <si>
+    <t> Berry Manilow sour; Looks Good on You Though hazy IPA;</t>
+  </si>
+  <si>
+    <t> Cloud Candy hazy IPA; Sour Face</t>
+  </si>
+  <si>
+    <t> Chimera fruited sour; Happy Learned to Putt DIPA; a surprise?!;</t>
+  </si>
+  <si>
+    <t> 2015 Barleywine; 2018 BA Russian Imperial Stout; Helles; Doppelbock;</t>
+  </si>
+  <si>
+    <t> NYIPA; Raspberry Lemon Kolsch;</t>
+  </si>
+  <si>
+    <t>  You Bet Your Dupa I’m Polish Grodziskie; NSB ESB; Get Bee to a Nunnery golden ale;</t>
+  </si>
+  <si>
+    <t> Citra Citra Citra NEIPA; Mise en Place</t>
+  </si>
+  <si>
+    <t> Bock on Wood (wood-aged Helles bock); Curuba Kolsch; Frisco Kid WC IPA;</t>
+  </si>
+  <si>
+    <t> Solo Exhibition</t>
+  </si>
+  <si>
+    <t> Full Rolling (Belgian white with sumo oranges); Tin Plate (chocolate raspberry stout aged in Cab Sauv barrel);</t>
+  </si>
+  <si>
+    <t> DDH Mass Riot IPA; Tangerine Wit; Hops Springs Eternal NYS lager; Dark in Daytime stout;</t>
+  </si>
+  <si>
+    <t> Nocturnal Pivo; 10th anniversary IPA; On the Tea iced tea lemonade sour;</t>
+  </si>
+  <si>
+    <t> Rhymenoceros New Zealand Pils; Infinite Citra dipa; Bumbleberry It Was Written sour IPA;</t>
+  </si>
+  <si>
+    <t> Helles, Sunset Sorbet, Nautical Mile and Sam Patch Porter;</t>
+  </si>
+  <si>
+    <t> Sager Landbier (German amber lager); University Ave Pale Ale; Jessica Rabbit Red WC red ale; Mr. Socko's Saison;</t>
+  </si>
+  <si>
+    <t> Azacca hop cider; Do you like jazz (braggot);</t>
+  </si>
+  <si>
+    <t> Horse with no Name (barrel-fermented Flanders-inspired sour brown); Rauchbier smoked amber lager; Biere de Mars (clean) saison;</t>
+  </si>
+  <si>
+    <t> Olney in NY hazy IPA; TBA;</t>
+  </si>
+  <si>
+    <t>  Strike Anywhere lager; Chaos by Design imperial stout (Mortalis collab); Neck Breaker (Metal Injection collab); Mass Delusion hazy IPA;</t>
+  </si>
+  <si>
+    <t> Yes... A Pudding Beer (Note</t>
+  </si>
+  <si>
+    <t> ESB cask; Pucker up Sweetie hibiscus punch sour;</t>
+  </si>
+  <si>
+    <t> Salus saison; Unfettered Soul hazy DIPA; Whale Herder cream ale; Blackbird IPA collab;</t>
+  </si>
+  <si>
+    <t> Polotmavy Pivo; Is This Beer? Raspberry Lime sour; Swifty Shifty light lager; Makin' Waves hazy pale;</t>
+  </si>
+  <si>
+    <t> Bone Twig NE pale; Bone Tree NEIPA; Selected 4th Anniversary DIPA;</t>
+  </si>
+  <si>
+    <t> Barrel-Aged Baltic porter; Seabreeze Summer Ale;</t>
+  </si>
+  <si>
+    <t> Graffiti Highway IPA; Freaky Squeeze spiked lemonade;</t>
+  </si>
+  <si>
+    <t> TBA (but I guarantee it will be delicious);</t>
+  </si>
+  <si>
+    <t> Vienna Classic Vienna lager; Mild Lockout Munich-style Helles lager;</t>
+  </si>
+  <si>
+    <t> Variable IPA; Vast Expanse hazy IPA; Conceptual DIPA;</t>
+  </si>
+  <si>
+    <t> TBA;</t>
+  </si>
+  <si>
+    <t> Grodziskie; Outskirts hazy pale ale;</t>
+  </si>
+  <si>
+    <t> L’Ultima Moda Italian Pilsner, Prudence English Mild, First Pitch American Pale Ale, TBA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">903 Beer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angry Chair </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aporia Coffee </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ardennes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arkane </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Athletic Brewing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aurora </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Badlands </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beelzebubbles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big Ditch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birdhouse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlackBird </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blood Brothers </t>
+  </si>
+  <si>
+    <t>Brewlihan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BriarBrothers </t>
+  </si>
+  <si>
+    <t>Bright Path </t>
+  </si>
+  <si>
+    <t>Bullfinch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celestial </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cinderlands </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counterpart </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dancing Gnome </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dewey </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eli Fish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Embark Cider </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eredita </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faircraft </t>
+  </si>
+  <si>
+    <t>Fidens </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fifth Frame </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finback </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequentem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Froth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genesee </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grimm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happy Gut </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heavy Reel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human Robot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illumination Mead </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imprint </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Tug </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irondequoit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jack's Abby </t>
+  </si>
+  <si>
+    <t xml:space="preserve">K2 Brothers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katboocha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kettlehead </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knucklehead </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laurentide </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Living Roots </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lock 32 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnanimous </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masthead </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matron </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meier's Creek </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mighty Squirrel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortalis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naked Dove </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naples </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nine Spot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noble Shepherd </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Okay </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old Thunder </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Half </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preservation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prison City </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resurgence </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rising Storm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohrbach </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sager </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seed + Stone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver Lake </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sloop </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smoldered Society </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stoneyard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strange Design </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strangebird </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swiftwater </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third Moon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three Heads </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Troegs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trophy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">True History </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Underground Beer Lab </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wayland </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wayward Lane </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wild East </t>
+  </si>
+  <si>
+    <t>Genesee branded stand near main entrance</t>
+  </si>
+  <si>
+    <t>Rohrbach branded stand near main entrance</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Subsection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -501,6 +1045,21 @@
       <color rgb="FF404040"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF363737"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -523,9 +1082,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,10 +1406,1235 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4B1671-580F-0B4D-9A65-DA210F75C570}">
+  <dimension ref="A1:E86"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="38" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" s="3">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C3" s="3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C4" s="3">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C10" s="3">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C11" s="3">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C12" s="3">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C15" s="3">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C16" s="3">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C17" s="3">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C18" s="3">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C19" s="3">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C22" s="3">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C23" s="3">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C24" s="3">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C25" s="3">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C26" s="3">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C27" s="3">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C28" s="3">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C29" s="3">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C30" s="3">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C31" s="3">
+        <v>18</v>
+      </c>
+      <c r="D31" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C32" s="3">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C34" s="3">
+        <v>19</v>
+      </c>
+      <c r="D34" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C35" s="3">
+        <v>17</v>
+      </c>
+      <c r="D35" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C36" s="3">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C37" s="3">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C38" s="3">
+        <v>16</v>
+      </c>
+      <c r="D38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C39" s="3">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>186</v>
+      </c>
+      <c r="E39" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C42" s="3">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C43" s="3">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C44" s="3">
+        <v>11</v>
+      </c>
+      <c r="D44" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C45" s="3">
+        <v>16</v>
+      </c>
+      <c r="D45" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C46" s="3">
+        <v>15</v>
+      </c>
+      <c r="D46" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C47" s="3">
+        <v>12</v>
+      </c>
+      <c r="D47" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C48" s="3">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C49" s="3">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C50" s="3">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C51" s="3">
+        <v>14</v>
+      </c>
+      <c r="D51" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C52" s="3">
+        <v>9</v>
+      </c>
+      <c r="D52" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C53" s="3">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C54" s="3">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C55" s="3">
+        <v>2</v>
+      </c>
+      <c r="D55" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C56" s="3">
+        <v>23</v>
+      </c>
+      <c r="D56" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C57" s="3">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C58" s="3">
+        <v>11</v>
+      </c>
+      <c r="D58" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C59" s="3">
+        <v>12</v>
+      </c>
+      <c r="D59" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C60" s="3">
+        <v>5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C61" s="3">
+        <v>14</v>
+      </c>
+      <c r="D61" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C62" s="3">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C63" s="3">
+        <v>8</v>
+      </c>
+      <c r="D63" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C64" s="3">
+        <v>3</v>
+      </c>
+      <c r="D64" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C65" s="3">
+        <v>9</v>
+      </c>
+      <c r="D65" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C66" s="3">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C67" s="3">
+        <v>18</v>
+      </c>
+      <c r="D67" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="D68" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C69" s="3">
+        <v>20</v>
+      </c>
+      <c r="D69" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C70" s="3">
+        <v>13</v>
+      </c>
+      <c r="D70" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C71" s="3">
+        <v>10</v>
+      </c>
+      <c r="D71" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C72" s="3">
+        <v>6</v>
+      </c>
+      <c r="D72" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C73" s="3">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C74" s="3">
+        <v>22</v>
+      </c>
+      <c r="D74" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C75" s="3">
+        <v>14</v>
+      </c>
+      <c r="D75" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C76" s="3">
+        <v>7</v>
+      </c>
+      <c r="D76" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C77" s="3">
+        <v>6</v>
+      </c>
+      <c r="D77" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C78" s="3">
+        <v>5</v>
+      </c>
+      <c r="D78" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C79" s="3">
+        <v>13</v>
+      </c>
+      <c r="D79" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C80" s="3">
+        <v>10</v>
+      </c>
+      <c r="D80" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C81" s="3">
+        <v>7</v>
+      </c>
+      <c r="D81" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C82" s="3">
+        <v>7</v>
+      </c>
+      <c r="D82" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C83" s="3">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C84" s="3">
+        <v>8</v>
+      </c>
+      <c r="D84" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C85" s="3">
+        <v>6</v>
+      </c>
+      <c r="D85" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C86" s="3">
+        <v>6</v>
+      </c>
+      <c r="D86" t="s">
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F21ACD-7CC6-814B-B570-189F2A313E51}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>